<commit_message>
- Implemented very barebones of monster framework - Sorted AI class, now each AI instance is unique rather than static - Tweaks in interaction, and entity facing - Overhauled the interaction system, the cursor system is a little buggy still - Centered minimap icons (and icons in buttons in general)
</commit_message>
<xml_diff>
--- a/data_raw/stat_growth.xlsx
+++ b/data_raw/stat_growth.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="11140" yWindow="0" windowWidth="25600" windowHeight="15120" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="18">
   <si>
     <t>Warrior</t>
   </si>
@@ -44,6 +44,36 @@
   <si>
     <t>EXP</t>
   </si>
+  <si>
+    <t>Strength</t>
+  </si>
+  <si>
+    <t>Lv.</t>
+  </si>
+  <si>
+    <t>Dexterity</t>
+  </si>
+  <si>
+    <t>Intelligence</t>
+  </si>
+  <si>
+    <t>Luck</t>
+  </si>
+  <si>
+    <t>Speed</t>
+  </si>
+  <si>
+    <t>MAX: 50</t>
+  </si>
+  <si>
+    <t>MAX: 35</t>
+  </si>
+  <si>
+    <t>MAX: 30</t>
+  </si>
+  <si>
+    <t>MAX: 15</t>
+  </si>
 </sst>
 </file>
 
@@ -55,7 +85,6 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="136"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -111,7 +140,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -181,8 +210,56 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="9">
+  <cellStyleXfs count="11">
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="1" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -192,8 +269,10 @@
     <xf numFmtId="1" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="1" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="22">
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -210,16 +289,24 @@
     <xf numFmtId="1" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="9">
+  <cellStyles count="11">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -549,10 +636,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J62"/>
+  <dimension ref="A1:P64"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="B45" workbookViewId="0">
-      <selection activeCell="J62" sqref="J3:J62"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="E29" workbookViewId="0">
+      <selection activeCell="Q50" sqref="Q50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -566,9 +653,14 @@
     <col min="8" max="8" width="10.83203125" style="7"/>
     <col min="9" max="9" width="10.83203125" style="9"/>
     <col min="10" max="10" width="10.83203125" style="14"/>
+    <col min="12" max="12" width="10.83203125" style="1"/>
+    <col min="13" max="13" width="10.83203125" style="19"/>
+    <col min="14" max="14" width="10.83203125" style="2"/>
+    <col min="15" max="15" width="10.83203125" style="20"/>
+    <col min="16" max="16" width="10.83203125" style="19"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:16">
       <c r="A1" s="2"/>
       <c r="B1" s="4" t="s">
         <v>0</v>
@@ -583,8 +675,13 @@
       <c r="H1" s="7" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:10">
+      <c r="L1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M1" s="17"/>
+      <c r="P1" s="17"/>
+    </row>
+    <row r="2" spans="1:16">
       <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
@@ -615,8 +712,26 @@
       <c r="J2" s="15" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:10">
+      <c r="K2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="L2" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="M2" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="O2" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="P2" s="18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -656,8 +771,31 @@
         <f>(A3 *10)^2 +2^A3/(A3^6)</f>
         <v>102</v>
       </c>
-    </row>
-    <row r="4" spans="1:10">
+      <c r="K3" s="1">
+        <v>1</v>
+      </c>
+      <c r="L3" s="1">
+        <f>5+(A3-1)/2</f>
+        <v>5</v>
+      </c>
+      <c r="M3" s="19">
+        <f>2+(A3-1)/4</f>
+        <v>2</v>
+      </c>
+      <c r="N3" s="2">
+        <f>1+(A3-2)/6</f>
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="O3" s="20">
+        <f>0+(A3-1)/10</f>
+        <v>0</v>
+      </c>
+      <c r="P3" s="19">
+        <f>10+(A3-1)/8</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -670,7 +808,7 @@
         <v>9.3076923076923084</v>
       </c>
       <c r="D4" s="12">
-        <f t="shared" ref="D4:D62" si="2">17+A4+A4^2/4</f>
+        <f t="shared" ref="D4:D61" si="2">17+A4+A4^2/4</f>
         <v>20</v>
       </c>
       <c r="E4" s="13">
@@ -697,8 +835,31 @@
         <f t="shared" ref="J4:J62" si="8">(A4 *10)^2 +2^A4/(A4^6)</f>
         <v>400.0625</v>
       </c>
-    </row>
-    <row r="5" spans="1:10">
+      <c r="K4" s="1">
+        <v>2</v>
+      </c>
+      <c r="L4" s="1">
+        <f t="shared" ref="L4:L62" si="9">5+(A4-1)/2</f>
+        <v>5.5</v>
+      </c>
+      <c r="M4" s="19">
+        <f t="shared" ref="M4:M62" si="10">2+(A4-1)/4</f>
+        <v>2.25</v>
+      </c>
+      <c r="N4" s="2">
+        <f t="shared" ref="N4:N62" si="11">1+(A4-2)/6</f>
+        <v>1</v>
+      </c>
+      <c r="O4" s="20">
+        <f t="shared" ref="O4:O62" si="12">0+(A4-1)/10</f>
+        <v>0.1</v>
+      </c>
+      <c r="P4" s="19">
+        <f t="shared" ref="P4:P62" si="13">10+(A4-1)/8</f>
+        <v>10.125</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -738,8 +899,31 @@
         <f t="shared" si="8"/>
         <v>900.01097393689986</v>
       </c>
-    </row>
-    <row r="6" spans="1:10">
+      <c r="K5" s="1">
+        <v>3</v>
+      </c>
+      <c r="L5" s="1">
+        <f t="shared" si="9"/>
+        <v>6</v>
+      </c>
+      <c r="M5" s="19">
+        <f t="shared" si="10"/>
+        <v>2.5</v>
+      </c>
+      <c r="N5" s="2">
+        <f t="shared" si="11"/>
+        <v>1.1666666666666667</v>
+      </c>
+      <c r="O5" s="20">
+        <f t="shared" si="12"/>
+        <v>0.2</v>
+      </c>
+      <c r="P5" s="19">
+        <f t="shared" si="13"/>
+        <v>10.25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -779,8 +963,31 @@
         <f t="shared" si="8"/>
         <v>1600.00390625</v>
       </c>
-    </row>
-    <row r="7" spans="1:10">
+      <c r="K6" s="1">
+        <v>4</v>
+      </c>
+      <c r="L6" s="1">
+        <f t="shared" si="9"/>
+        <v>6.5</v>
+      </c>
+      <c r="M6" s="19">
+        <f t="shared" si="10"/>
+        <v>2.75</v>
+      </c>
+      <c r="N6" s="2">
+        <f t="shared" si="11"/>
+        <v>1.3333333333333333</v>
+      </c>
+      <c r="O6" s="20">
+        <f t="shared" si="12"/>
+        <v>0.3</v>
+      </c>
+      <c r="P6" s="19">
+        <f t="shared" si="13"/>
+        <v>10.375</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -820,8 +1027,31 @@
         <f t="shared" si="8"/>
         <v>2500.0020479999998</v>
       </c>
-    </row>
-    <row r="8" spans="1:10">
+      <c r="K7" s="1">
+        <v>5</v>
+      </c>
+      <c r="L7" s="1">
+        <f t="shared" si="9"/>
+        <v>7</v>
+      </c>
+      <c r="M7" s="19">
+        <f t="shared" si="10"/>
+        <v>3</v>
+      </c>
+      <c r="N7" s="2">
+        <f t="shared" si="11"/>
+        <v>1.5</v>
+      </c>
+      <c r="O7" s="20">
+        <f t="shared" si="12"/>
+        <v>0.4</v>
+      </c>
+      <c r="P7" s="19">
+        <f t="shared" si="13"/>
+        <v>10.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -861,8 +1091,31 @@
         <f t="shared" si="8"/>
         <v>3600.0013717421125</v>
       </c>
-    </row>
-    <row r="9" spans="1:10">
+      <c r="K8" s="1">
+        <v>6</v>
+      </c>
+      <c r="L8" s="1">
+        <f t="shared" si="9"/>
+        <v>7.5</v>
+      </c>
+      <c r="M8" s="19">
+        <f t="shared" si="10"/>
+        <v>3.25</v>
+      </c>
+      <c r="N8" s="2">
+        <f t="shared" si="11"/>
+        <v>1.6666666666666665</v>
+      </c>
+      <c r="O8" s="20">
+        <f t="shared" si="12"/>
+        <v>0.5</v>
+      </c>
+      <c r="P8" s="19">
+        <f t="shared" si="13"/>
+        <v>10.625</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -902,8 +1155,31 @@
         <f t="shared" si="8"/>
         <v>4900.0010879820484</v>
       </c>
-    </row>
-    <row r="10" spans="1:10">
+      <c r="K9" s="1">
+        <v>7</v>
+      </c>
+      <c r="L9" s="1">
+        <f t="shared" si="9"/>
+        <v>8</v>
+      </c>
+      <c r="M9" s="19">
+        <f t="shared" si="10"/>
+        <v>3.5</v>
+      </c>
+      <c r="N9" s="2">
+        <f t="shared" si="11"/>
+        <v>1.8333333333333335</v>
+      </c>
+      <c r="O9" s="20">
+        <f t="shared" si="12"/>
+        <v>0.6</v>
+      </c>
+      <c r="P9" s="19">
+        <f t="shared" si="13"/>
+        <v>10.75</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -943,8 +1219,31 @@
         <f t="shared" si="8"/>
         <v>6400.0009765625</v>
       </c>
-    </row>
-    <row r="11" spans="1:10">
+      <c r="K10" s="1">
+        <v>8</v>
+      </c>
+      <c r="L10" s="1">
+        <f t="shared" si="9"/>
+        <v>8.5</v>
+      </c>
+      <c r="M10" s="19">
+        <f t="shared" si="10"/>
+        <v>3.75</v>
+      </c>
+      <c r="N10" s="2">
+        <f t="shared" si="11"/>
+        <v>2</v>
+      </c>
+      <c r="O10" s="20">
+        <f t="shared" si="12"/>
+        <v>0.7</v>
+      </c>
+      <c r="P10" s="19">
+        <f t="shared" si="13"/>
+        <v>10.875</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -953,7 +1252,7 @@
         <v>54</v>
       </c>
       <c r="C11" s="13">
-        <f t="shared" ref="C11:C62" si="9">7 + A11 + A11^2 / 13</f>
+        <f t="shared" ref="C11:C62" si="14">7 + A11 + A11^2 / 13</f>
         <v>22.23076923076923</v>
       </c>
       <c r="D11" s="12">
@@ -965,11 +1264,11 @@
         <v>28</v>
       </c>
       <c r="F11" s="12">
-        <f t="shared" ref="F11:F62" si="10">16 + A11 + A11^2 / 5</f>
+        <f t="shared" ref="F11:F62" si="15">16 + A11 + A11^2 / 5</f>
         <v>41.2</v>
       </c>
       <c r="G11" s="13">
-        <f t="shared" ref="G11:G62" si="11">8+A11 + 2 +A11^2 / 4</f>
+        <f t="shared" ref="G11:G62" si="16">8+A11 + 2 +A11^2 / 4</f>
         <v>39.25</v>
       </c>
       <c r="H11" s="12">
@@ -984,8 +1283,31 @@
         <f t="shared" si="8"/>
         <v>8100.0009634183289</v>
       </c>
-    </row>
-    <row r="12" spans="1:10">
+      <c r="K11" s="1">
+        <v>9</v>
+      </c>
+      <c r="L11" s="1">
+        <f t="shared" si="9"/>
+        <v>9</v>
+      </c>
+      <c r="M11" s="19">
+        <f t="shared" si="10"/>
+        <v>4</v>
+      </c>
+      <c r="N11" s="2">
+        <f t="shared" si="11"/>
+        <v>2.166666666666667</v>
+      </c>
+      <c r="O11" s="20">
+        <f t="shared" si="12"/>
+        <v>0.8</v>
+      </c>
+      <c r="P11" s="19">
+        <f t="shared" si="13"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -994,7 +1316,7 @@
         <v>61.333333333333336</v>
       </c>
       <c r="C12" s="13">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>24.692307692307693</v>
       </c>
       <c r="D12" s="12">
@@ -1006,11 +1328,11 @@
         <v>31.111111111111111</v>
       </c>
       <c r="F12" s="12">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>46</v>
       </c>
       <c r="G12" s="13">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>45</v>
       </c>
       <c r="H12" s="12">
@@ -1025,8 +1347,31 @@
         <f t="shared" si="8"/>
         <v>10000.001023999999</v>
       </c>
-    </row>
-    <row r="13" spans="1:10">
+      <c r="K12" s="1">
+        <v>10</v>
+      </c>
+      <c r="L12" s="1">
+        <f t="shared" si="9"/>
+        <v>9.5</v>
+      </c>
+      <c r="M12" s="19">
+        <f t="shared" si="10"/>
+        <v>4.25</v>
+      </c>
+      <c r="N12" s="2">
+        <f t="shared" si="11"/>
+        <v>2.333333333333333</v>
+      </c>
+      <c r="O12" s="20">
+        <f t="shared" si="12"/>
+        <v>0.9</v>
+      </c>
+      <c r="P12" s="19">
+        <f t="shared" si="13"/>
+        <v>11.125</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -1035,7 +1380,7 @@
         <v>69.333333333333343</v>
       </c>
       <c r="C13" s="13">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>27.307692307692307</v>
       </c>
       <c r="D13" s="12">
@@ -1047,11 +1392,11 @@
         <v>34.444444444444443</v>
       </c>
       <c r="F13" s="12">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>51.2</v>
       </c>
       <c r="G13" s="13">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>51.25</v>
       </c>
       <c r="H13" s="12">
@@ -1066,8 +1411,31 @@
         <f t="shared" si="8"/>
         <v>12100.001156042608</v>
       </c>
-    </row>
-    <row r="14" spans="1:10">
+      <c r="K13" s="1">
+        <v>11</v>
+      </c>
+      <c r="L13" s="1">
+        <f t="shared" si="9"/>
+        <v>10</v>
+      </c>
+      <c r="M13" s="19">
+        <f t="shared" si="10"/>
+        <v>4.5</v>
+      </c>
+      <c r="N13" s="2">
+        <f t="shared" si="11"/>
+        <v>2.5</v>
+      </c>
+      <c r="O13" s="20">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+      <c r="P13" s="19">
+        <f t="shared" si="13"/>
+        <v>11.25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -1076,7 +1444,7 @@
         <v>78</v>
       </c>
       <c r="C14" s="13">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>30.076923076923077</v>
       </c>
       <c r="D14" s="12">
@@ -1088,11 +1456,11 @@
         <v>38</v>
       </c>
       <c r="F14" s="12">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>56.8</v>
       </c>
       <c r="G14" s="13">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>58</v>
       </c>
       <c r="H14" s="12">
@@ -1107,8 +1475,31 @@
         <f t="shared" si="8"/>
         <v>14400.001371742112</v>
       </c>
-    </row>
-    <row r="15" spans="1:10">
+      <c r="K14" s="1">
+        <v>12</v>
+      </c>
+      <c r="L14" s="1">
+        <f t="shared" si="9"/>
+        <v>10.5</v>
+      </c>
+      <c r="M14" s="19">
+        <f t="shared" si="10"/>
+        <v>4.75</v>
+      </c>
+      <c r="N14" s="2">
+        <f t="shared" si="11"/>
+        <v>2.666666666666667</v>
+      </c>
+      <c r="O14" s="20">
+        <f t="shared" si="12"/>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="P14" s="19">
+        <f t="shared" si="13"/>
+        <v>11.375</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -1117,7 +1508,7 @@
         <v>87.333333333333343</v>
       </c>
       <c r="C15" s="13">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>33</v>
       </c>
       <c r="D15" s="12">
@@ -1129,11 +1520,11 @@
         <v>41.777777777777779</v>
       </c>
       <c r="F15" s="12">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>62.8</v>
       </c>
       <c r="G15" s="13">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>65.25</v>
       </c>
       <c r="H15" s="12">
@@ -1148,8 +1539,31 @@
         <f t="shared" si="8"/>
         <v>16900.001697187519</v>
       </c>
-    </row>
-    <row r="16" spans="1:10">
+      <c r="K15" s="1">
+        <v>13</v>
+      </c>
+      <c r="L15" s="1">
+        <f t="shared" si="9"/>
+        <v>11</v>
+      </c>
+      <c r="M15" s="19">
+        <f t="shared" si="10"/>
+        <v>5</v>
+      </c>
+      <c r="N15" s="2">
+        <f t="shared" si="11"/>
+        <v>2.833333333333333</v>
+      </c>
+      <c r="O15" s="20">
+        <f t="shared" si="12"/>
+        <v>1.2</v>
+      </c>
+      <c r="P15" s="19">
+        <f t="shared" si="13"/>
+        <v>11.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -1158,7 +1572,7 @@
         <v>97.333333333333329</v>
       </c>
       <c r="C16" s="13">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>36.07692307692308</v>
       </c>
       <c r="D16" s="12">
@@ -1170,11 +1584,11 @@
         <v>45.777777777777779</v>
       </c>
       <c r="F16" s="12">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>69.2</v>
       </c>
       <c r="G16" s="13">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>73</v>
       </c>
       <c r="H16" s="12">
@@ -1189,8 +1603,31 @@
         <f t="shared" si="8"/>
         <v>19600.002175964095</v>
       </c>
-    </row>
-    <row r="17" spans="1:10">
+      <c r="K16" s="1">
+        <v>14</v>
+      </c>
+      <c r="L16" s="1">
+        <f t="shared" si="9"/>
+        <v>11.5</v>
+      </c>
+      <c r="M16" s="19">
+        <f t="shared" si="10"/>
+        <v>5.25</v>
+      </c>
+      <c r="N16" s="2">
+        <f t="shared" si="11"/>
+        <v>3</v>
+      </c>
+      <c r="O16" s="20">
+        <f t="shared" si="12"/>
+        <v>1.3</v>
+      </c>
+      <c r="P16" s="19">
+        <f t="shared" si="13"/>
+        <v>11.625</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -1199,7 +1636,7 @@
         <v>108</v>
       </c>
       <c r="C17" s="13">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>39.307692307692307</v>
       </c>
       <c r="D17" s="12">
@@ -1211,27 +1648,50 @@
         <v>50</v>
       </c>
       <c r="F17" s="12">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>76</v>
       </c>
       <c r="G17" s="13">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>81.25</v>
       </c>
       <c r="H17" s="12">
-        <f t="shared" ref="H17:H34" si="12">14+A17+A17^2/10</f>
+        <f t="shared" ref="H17:H34" si="17">14+A17+A17^2/10</f>
         <v>51.5</v>
       </c>
       <c r="I17" s="13">
-        <f t="shared" ref="I17:I34" si="13">16+A17+1+A17^2/2</f>
+        <f t="shared" ref="I17:I34" si="18">16+A17+1+A17^2/2</f>
         <v>144.5</v>
       </c>
       <c r="J17" s="14">
         <f t="shared" si="8"/>
         <v>22500.002876751714</v>
       </c>
-    </row>
-    <row r="18" spans="1:10">
+      <c r="K17" s="1">
+        <v>15</v>
+      </c>
+      <c r="L17" s="1">
+        <f t="shared" si="9"/>
+        <v>12</v>
+      </c>
+      <c r="M17" s="19">
+        <f t="shared" si="10"/>
+        <v>5.5</v>
+      </c>
+      <c r="N17" s="2">
+        <f t="shared" si="11"/>
+        <v>3.1666666666666665</v>
+      </c>
+      <c r="O17" s="20">
+        <f t="shared" si="12"/>
+        <v>1.4</v>
+      </c>
+      <c r="P17" s="19">
+        <f t="shared" si="13"/>
+        <v>11.75</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -1240,7 +1700,7 @@
         <v>119.33333333333333</v>
       </c>
       <c r="C18" s="13">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>42.692307692307693</v>
       </c>
       <c r="D18" s="12">
@@ -1252,27 +1712,50 @@
         <v>54.444444444444443</v>
       </c>
       <c r="F18" s="12">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>83.2</v>
       </c>
       <c r="G18" s="13">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>90</v>
       </c>
       <c r="H18" s="12">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v>55.6</v>
       </c>
       <c r="I18" s="13">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>161</v>
       </c>
       <c r="J18" s="14">
         <f t="shared" si="8"/>
         <v>25600.00390625</v>
       </c>
-    </row>
-    <row r="19" spans="1:10">
+      <c r="K18" s="1">
+        <v>16</v>
+      </c>
+      <c r="L18" s="1">
+        <f t="shared" si="9"/>
+        <v>12.5</v>
+      </c>
+      <c r="M18" s="19">
+        <f t="shared" si="10"/>
+        <v>5.75</v>
+      </c>
+      <c r="N18" s="2">
+        <f t="shared" si="11"/>
+        <v>3.3333333333333335</v>
+      </c>
+      <c r="O18" s="20">
+        <f t="shared" si="12"/>
+        <v>1.5</v>
+      </c>
+      <c r="P18" s="19">
+        <f t="shared" si="13"/>
+        <v>11.875</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -1281,7 +1764,7 @@
         <v>131.33333333333331</v>
       </c>
       <c r="C19" s="13">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>46.230769230769226</v>
       </c>
       <c r="D19" s="12">
@@ -1293,27 +1776,50 @@
         <v>59.111111111111114</v>
       </c>
       <c r="F19" s="12">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>90.8</v>
       </c>
       <c r="G19" s="13">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>99.25</v>
       </c>
       <c r="H19" s="12">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v>59.9</v>
       </c>
       <c r="I19" s="13">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>178.5</v>
       </c>
       <c r="J19" s="14">
         <f t="shared" si="8"/>
         <v>28900.005430207158</v>
       </c>
-    </row>
-    <row r="20" spans="1:10">
+      <c r="K19" s="1">
+        <v>17</v>
+      </c>
+      <c r="L19" s="1">
+        <f t="shared" si="9"/>
+        <v>13</v>
+      </c>
+      <c r="M19" s="19">
+        <f t="shared" si="10"/>
+        <v>6</v>
+      </c>
+      <c r="N19" s="2">
+        <f t="shared" si="11"/>
+        <v>3.5</v>
+      </c>
+      <c r="O19" s="20">
+        <f t="shared" si="12"/>
+        <v>1.6</v>
+      </c>
+      <c r="P19" s="19">
+        <f t="shared" si="13"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -1322,7 +1828,7 @@
         <v>144</v>
       </c>
       <c r="C20" s="13">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>49.92307692307692</v>
       </c>
       <c r="D20" s="12">
@@ -1334,27 +1840,50 @@
         <v>64</v>
       </c>
       <c r="F20" s="12">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>98.8</v>
       </c>
       <c r="G20" s="13">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>109</v>
       </c>
       <c r="H20" s="12">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v>64.400000000000006</v>
       </c>
       <c r="I20" s="13">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>197</v>
       </c>
       <c r="J20" s="14">
         <f t="shared" si="8"/>
         <v>32400.007707346631</v>
       </c>
-    </row>
-    <row r="21" spans="1:10">
+      <c r="K20" s="1">
+        <v>18</v>
+      </c>
+      <c r="L20" s="1">
+        <f t="shared" si="9"/>
+        <v>13.5</v>
+      </c>
+      <c r="M20" s="19">
+        <f t="shared" si="10"/>
+        <v>6.25</v>
+      </c>
+      <c r="N20" s="2">
+        <f t="shared" si="11"/>
+        <v>3.6666666666666665</v>
+      </c>
+      <c r="O20" s="20">
+        <f t="shared" si="12"/>
+        <v>1.7</v>
+      </c>
+      <c r="P20" s="19">
+        <f t="shared" si="13"/>
+        <v>12.125</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -1363,7 +1892,7 @@
         <v>157.33333333333331</v>
       </c>
       <c r="C21" s="13">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>53.769230769230774</v>
       </c>
       <c r="D21" s="12">
@@ -1375,27 +1904,50 @@
         <v>69.111111111111114</v>
       </c>
       <c r="F21" s="12">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>107.2</v>
       </c>
       <c r="G21" s="13">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>119.25</v>
       </c>
       <c r="H21" s="12">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v>69.099999999999994</v>
       </c>
       <c r="I21" s="13">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>216.5</v>
       </c>
       <c r="J21" s="14">
         <f t="shared" si="8"/>
         <v>36100.011144184973</v>
       </c>
-    </row>
-    <row r="22" spans="1:10">
+      <c r="K21" s="1">
+        <v>19</v>
+      </c>
+      <c r="L21" s="1">
+        <f t="shared" si="9"/>
+        <v>14</v>
+      </c>
+      <c r="M21" s="19">
+        <f t="shared" si="10"/>
+        <v>6.5</v>
+      </c>
+      <c r="N21" s="2">
+        <f t="shared" si="11"/>
+        <v>3.8333333333333335</v>
+      </c>
+      <c r="O21" s="20">
+        <f t="shared" si="12"/>
+        <v>1.8</v>
+      </c>
+      <c r="P21" s="19">
+        <f t="shared" si="13"/>
+        <v>12.25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -1404,7 +1956,7 @@
         <v>171.33333333333334</v>
       </c>
       <c r="C22" s="13">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>57.769230769230774</v>
       </c>
       <c r="D22" s="12">
@@ -1416,27 +1968,50 @@
         <v>74.444444444444443</v>
       </c>
       <c r="F22" s="12">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>116</v>
       </c>
       <c r="G22" s="13">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>130</v>
       </c>
       <c r="H22" s="12">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v>74</v>
       </c>
       <c r="I22" s="13">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>237</v>
       </c>
       <c r="J22" s="14">
         <f t="shared" si="8"/>
         <v>40000.016384000002</v>
       </c>
-    </row>
-    <row r="23" spans="1:10">
+      <c r="K22" s="1">
+        <v>20</v>
+      </c>
+      <c r="L22" s="1">
+        <f t="shared" si="9"/>
+        <v>14.5</v>
+      </c>
+      <c r="M22" s="19">
+        <f t="shared" si="10"/>
+        <v>6.75</v>
+      </c>
+      <c r="N22" s="2">
+        <f t="shared" si="11"/>
+        <v>4</v>
+      </c>
+      <c r="O22" s="20">
+        <f t="shared" si="12"/>
+        <v>1.9</v>
+      </c>
+      <c r="P22" s="19">
+        <f t="shared" si="13"/>
+        <v>12.375</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -1445,7 +2020,7 @@
         <v>186</v>
       </c>
       <c r="C23" s="13">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>61.92307692307692</v>
       </c>
       <c r="D23" s="12">
@@ -1457,27 +2032,50 @@
         <v>80</v>
       </c>
       <c r="F23" s="12">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>125.2</v>
       </c>
       <c r="G23" s="13">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>141.25</v>
       </c>
       <c r="H23" s="12">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v>79.099999999999994</v>
       </c>
       <c r="I23" s="13">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>258.5</v>
       </c>
       <c r="J23" s="14">
         <f t="shared" si="8"/>
         <v>44100.024451986115</v>
       </c>
-    </row>
-    <row r="24" spans="1:10">
+      <c r="K23" s="1">
+        <v>21</v>
+      </c>
+      <c r="L23" s="1">
+        <f t="shared" si="9"/>
+        <v>15</v>
+      </c>
+      <c r="M23" s="19">
+        <f t="shared" si="10"/>
+        <v>7</v>
+      </c>
+      <c r="N23" s="2">
+        <f t="shared" si="11"/>
+        <v>4.1666666666666661</v>
+      </c>
+      <c r="O23" s="20">
+        <f t="shared" si="12"/>
+        <v>2</v>
+      </c>
+      <c r="P23" s="19">
+        <f t="shared" si="13"/>
+        <v>12.5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -1486,7 +2084,7 @@
         <v>201.33333333333334</v>
       </c>
       <c r="C24" s="13">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>66.230769230769226</v>
       </c>
       <c r="D24" s="12">
@@ -1498,27 +2096,50 @@
         <v>85.777777777777771</v>
       </c>
       <c r="F24" s="12">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>134.80000000000001</v>
       </c>
       <c r="G24" s="13">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>153</v>
       </c>
       <c r="H24" s="12">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v>84.4</v>
       </c>
       <c r="I24" s="13">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>281</v>
       </c>
       <c r="J24" s="14">
         <f t="shared" si="8"/>
         <v>48400.036993363479</v>
       </c>
-    </row>
-    <row r="25" spans="1:10">
+      <c r="K24" s="1">
+        <v>22</v>
+      </c>
+      <c r="L24" s="1">
+        <f t="shared" si="9"/>
+        <v>15.5</v>
+      </c>
+      <c r="M24" s="19">
+        <f t="shared" si="10"/>
+        <v>7.25</v>
+      </c>
+      <c r="N24" s="2">
+        <f t="shared" si="11"/>
+        <v>4.3333333333333339</v>
+      </c>
+      <c r="O24" s="20">
+        <f t="shared" si="12"/>
+        <v>2.1</v>
+      </c>
+      <c r="P24" s="19">
+        <f t="shared" si="13"/>
+        <v>12.625</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -1527,7 +2148,7 @@
         <v>217.33333333333334</v>
       </c>
       <c r="C25" s="13">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>70.692307692307693</v>
       </c>
       <c r="D25" s="12">
@@ -1539,27 +2160,50 @@
         <v>91.777777777777771</v>
       </c>
       <c r="F25" s="12">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>144.80000000000001</v>
       </c>
       <c r="G25" s="13">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>165.25</v>
       </c>
       <c r="H25" s="12">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v>89.9</v>
       </c>
       <c r="I25" s="13">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>304.5</v>
       </c>
       <c r="J25" s="14">
         <f t="shared" si="8"/>
         <v>52900.056666042648</v>
       </c>
-    </row>
-    <row r="26" spans="1:10">
+      <c r="K25" s="1">
+        <v>23</v>
+      </c>
+      <c r="L25" s="1">
+        <f t="shared" si="9"/>
+        <v>16</v>
+      </c>
+      <c r="M25" s="19">
+        <f t="shared" si="10"/>
+        <v>7.5</v>
+      </c>
+      <c r="N25" s="2">
+        <f t="shared" si="11"/>
+        <v>4.5</v>
+      </c>
+      <c r="O25" s="20">
+        <f t="shared" si="12"/>
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="P25" s="19">
+        <f t="shared" si="13"/>
+        <v>12.75</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -1568,7 +2212,7 @@
         <v>234</v>
       </c>
       <c r="C26" s="13">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>75.307692307692307</v>
       </c>
       <c r="D26" s="12">
@@ -1580,27 +2224,50 @@
         <v>98</v>
       </c>
       <c r="F26" s="12">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>155.19999999999999</v>
       </c>
       <c r="G26" s="13">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>178</v>
       </c>
       <c r="H26" s="12">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v>95.6</v>
       </c>
       <c r="I26" s="13">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>329</v>
       </c>
       <c r="J26" s="14">
         <f t="shared" si="8"/>
         <v>57600.0877914952</v>
       </c>
-    </row>
-    <row r="27" spans="1:10">
+      <c r="K26" s="1">
+        <v>24</v>
+      </c>
+      <c r="L26" s="1">
+        <f t="shared" si="9"/>
+        <v>16.5</v>
+      </c>
+      <c r="M26" s="19">
+        <f t="shared" si="10"/>
+        <v>7.75</v>
+      </c>
+      <c r="N26" s="2">
+        <f t="shared" si="11"/>
+        <v>4.6666666666666661</v>
+      </c>
+      <c r="O26" s="20">
+        <f t="shared" si="12"/>
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="P26" s="19">
+        <f t="shared" si="13"/>
+        <v>12.875</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -1609,7 +2276,7 @@
         <v>251.33333333333334</v>
       </c>
       <c r="C27" s="13">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>80.07692307692308</v>
       </c>
       <c r="D27" s="12">
@@ -1621,27 +2288,50 @@
         <v>104.44444444444444</v>
       </c>
       <c r="F27" s="12">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>166</v>
       </c>
       <c r="G27" s="13">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>191.25</v>
       </c>
       <c r="H27" s="12">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v>101.5</v>
       </c>
       <c r="I27" s="13">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>354.5</v>
       </c>
       <c r="J27" s="14">
         <f t="shared" si="8"/>
         <v>62500.137438953469</v>
       </c>
-    </row>
-    <row r="28" spans="1:10">
+      <c r="K27" s="1">
+        <v>25</v>
+      </c>
+      <c r="L27" s="1">
+        <f t="shared" si="9"/>
+        <v>17</v>
+      </c>
+      <c r="M27" s="19">
+        <f t="shared" si="10"/>
+        <v>8</v>
+      </c>
+      <c r="N27" s="2">
+        <f t="shared" si="11"/>
+        <v>4.8333333333333339</v>
+      </c>
+      <c r="O27" s="20">
+        <f t="shared" si="12"/>
+        <v>2.4</v>
+      </c>
+      <c r="P27" s="19">
+        <f t="shared" si="13"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16">
       <c r="A28" s="1">
         <v>26</v>
       </c>
@@ -1650,7 +2340,7 @@
         <v>269.33333333333337</v>
       </c>
       <c r="C28" s="13">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>85</v>
       </c>
       <c r="D28" s="12">
@@ -1662,27 +2352,50 @@
         <v>111.11111111111111</v>
       </c>
       <c r="F28" s="12">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>177.2</v>
       </c>
       <c r="G28" s="13">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>205</v>
       </c>
       <c r="H28" s="12">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v>107.6</v>
       </c>
       <c r="I28" s="13">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>381</v>
       </c>
       <c r="J28" s="14">
         <f t="shared" si="8"/>
         <v>67600.217240002661</v>
       </c>
-    </row>
-    <row r="29" spans="1:10">
+      <c r="K28" s="1">
+        <v>26</v>
+      </c>
+      <c r="L28" s="1">
+        <f t="shared" si="9"/>
+        <v>17.5</v>
+      </c>
+      <c r="M28" s="19">
+        <f t="shared" si="10"/>
+        <v>8.25</v>
+      </c>
+      <c r="N28" s="2">
+        <f t="shared" si="11"/>
+        <v>5</v>
+      </c>
+      <c r="O28" s="20">
+        <f t="shared" si="12"/>
+        <v>2.5</v>
+      </c>
+      <c r="P28" s="19">
+        <f t="shared" si="13"/>
+        <v>13.125</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16">
       <c r="A29" s="1">
         <v>27</v>
       </c>
@@ -1691,7 +2404,7 @@
         <v>288</v>
       </c>
       <c r="C29" s="13">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>90.07692307692308</v>
       </c>
       <c r="D29" s="12">
@@ -1703,27 +2416,50 @@
         <v>118</v>
       </c>
       <c r="F29" s="12">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>188.8</v>
       </c>
       <c r="G29" s="13">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>219.25</v>
       </c>
       <c r="H29" s="12">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v>113.9</v>
       </c>
       <c r="I29" s="13">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>408.5</v>
       </c>
       <c r="J29" s="14">
         <f t="shared" si="8"/>
         <v>72900.346439416113</v>
       </c>
-    </row>
-    <row r="30" spans="1:10">
+      <c r="K29" s="1">
+        <v>27</v>
+      </c>
+      <c r="L29" s="1">
+        <f t="shared" si="9"/>
+        <v>18</v>
+      </c>
+      <c r="M29" s="19">
+        <f t="shared" si="10"/>
+        <v>8.5</v>
+      </c>
+      <c r="N29" s="2">
+        <f t="shared" si="11"/>
+        <v>5.166666666666667</v>
+      </c>
+      <c r="O29" s="20">
+        <f t="shared" si="12"/>
+        <v>2.6</v>
+      </c>
+      <c r="P29" s="19">
+        <f t="shared" si="13"/>
+        <v>13.25</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16">
       <c r="A30" s="1">
         <v>28</v>
       </c>
@@ -1732,7 +2468,7 @@
         <v>307.33333333333331</v>
       </c>
       <c r="C30" s="13">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>95.307692307692307</v>
       </c>
       <c r="D30" s="12">
@@ -1744,27 +2480,50 @@
         <v>125.11111111111111</v>
       </c>
       <c r="F30" s="12">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>200.8</v>
       </c>
       <c r="G30" s="13">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>234</v>
       </c>
       <c r="H30" s="12">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v>120.4</v>
       </c>
       <c r="I30" s="13">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>437</v>
       </c>
       <c r="J30" s="14">
         <f t="shared" si="8"/>
         <v>78400.557046808724</v>
       </c>
-    </row>
-    <row r="31" spans="1:10">
+      <c r="K30" s="1">
+        <v>28</v>
+      </c>
+      <c r="L30" s="1">
+        <f t="shared" si="9"/>
+        <v>18.5</v>
+      </c>
+      <c r="M30" s="19">
+        <f t="shared" si="10"/>
+        <v>8.75</v>
+      </c>
+      <c r="N30" s="2">
+        <f t="shared" si="11"/>
+        <v>5.333333333333333</v>
+      </c>
+      <c r="O30" s="20">
+        <f t="shared" si="12"/>
+        <v>2.7</v>
+      </c>
+      <c r="P30" s="19">
+        <f t="shared" si="13"/>
+        <v>13.375</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16">
       <c r="A31" s="1">
         <v>29</v>
       </c>
@@ -1773,7 +2532,7 @@
         <v>327.33333333333331</v>
       </c>
       <c r="C31" s="13">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>100.69230769230769</v>
       </c>
       <c r="D31" s="12">
@@ -1785,27 +2544,50 @@
         <v>132.44444444444446</v>
       </c>
       <c r="F31" s="12">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>213.2</v>
       </c>
       <c r="G31" s="13">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>249.25</v>
       </c>
       <c r="H31" s="12">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v>127.1</v>
       </c>
       <c r="I31" s="13">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>466.5</v>
       </c>
       <c r="J31" s="14">
         <f t="shared" si="8"/>
         <v>84100.902572063074</v>
       </c>
-    </row>
-    <row r="32" spans="1:10">
+      <c r="K31" s="1">
+        <v>29</v>
+      </c>
+      <c r="L31" s="1">
+        <f t="shared" si="9"/>
+        <v>19</v>
+      </c>
+      <c r="M31" s="19">
+        <f t="shared" si="10"/>
+        <v>9</v>
+      </c>
+      <c r="N31" s="2">
+        <f t="shared" si="11"/>
+        <v>5.5</v>
+      </c>
+      <c r="O31" s="20">
+        <f t="shared" si="12"/>
+        <v>2.8</v>
+      </c>
+      <c r="P31" s="19">
+        <f t="shared" si="13"/>
+        <v>13.5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16">
       <c r="A32" s="1">
         <v>30</v>
       </c>
@@ -1814,7 +2596,7 @@
         <v>348</v>
       </c>
       <c r="C32" s="13">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>106.23076923076923</v>
       </c>
       <c r="D32" s="12">
@@ -1826,27 +2608,50 @@
         <v>140</v>
       </c>
       <c r="F32" s="12">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>226</v>
       </c>
       <c r="G32" s="13">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>265</v>
       </c>
       <c r="H32" s="12">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v>134</v>
       </c>
       <c r="I32" s="13">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>497</v>
       </c>
       <c r="J32" s="14">
         <f t="shared" si="8"/>
         <v>90001.472896877909</v>
       </c>
-    </row>
-    <row r="33" spans="1:10">
+      <c r="K32" s="1">
+        <v>30</v>
+      </c>
+      <c r="L32" s="1">
+        <f t="shared" si="9"/>
+        <v>19.5</v>
+      </c>
+      <c r="M32" s="19">
+        <f t="shared" si="10"/>
+        <v>9.25</v>
+      </c>
+      <c r="N32" s="2">
+        <f t="shared" si="11"/>
+        <v>5.666666666666667</v>
+      </c>
+      <c r="O32" s="20">
+        <f t="shared" si="12"/>
+        <v>2.9</v>
+      </c>
+      <c r="P32" s="19">
+        <f t="shared" si="13"/>
+        <v>13.625</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16">
       <c r="A33" s="1">
         <v>31</v>
       </c>
@@ -1855,7 +2660,7 @@
         <v>369.33333333333331</v>
       </c>
       <c r="C33" s="13">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>111.92307692307692</v>
       </c>
       <c r="D33" s="12">
@@ -1867,27 +2672,50 @@
         <v>147.77777777777777</v>
       </c>
       <c r="F33" s="12">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>239.2</v>
       </c>
       <c r="G33" s="13">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>281.25</v>
       </c>
       <c r="H33" s="12">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v>141.1</v>
       </c>
       <c r="I33" s="13">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>528.5</v>
       </c>
       <c r="J33" s="14">
         <f t="shared" si="8"/>
         <v>96102.41968984915</v>
       </c>
-    </row>
-    <row r="34" spans="1:10">
+      <c r="K33" s="1">
+        <v>31</v>
+      </c>
+      <c r="L33" s="1">
+        <f t="shared" si="9"/>
+        <v>20</v>
+      </c>
+      <c r="M33" s="19">
+        <f t="shared" si="10"/>
+        <v>9.5</v>
+      </c>
+      <c r="N33" s="2">
+        <f t="shared" si="11"/>
+        <v>5.833333333333333</v>
+      </c>
+      <c r="O33" s="20">
+        <f t="shared" si="12"/>
+        <v>3</v>
+      </c>
+      <c r="P33" s="19">
+        <f t="shared" si="13"/>
+        <v>13.75</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16">
       <c r="A34" s="1">
         <v>32</v>
       </c>
@@ -1896,7 +2724,7 @@
         <v>391.33333333333331</v>
       </c>
       <c r="C34" s="13">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>117.76923076923077</v>
       </c>
       <c r="D34" s="12">
@@ -1908,27 +2736,50 @@
         <v>155.77777777777777</v>
       </c>
       <c r="F34" s="12">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>252.8</v>
       </c>
       <c r="G34" s="13">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>298</v>
       </c>
       <c r="H34" s="12">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v>148.4</v>
       </c>
       <c r="I34" s="13">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>561</v>
       </c>
       <c r="J34" s="14">
         <f t="shared" si="8"/>
         <v>102404</v>
       </c>
-    </row>
-    <row r="35" spans="1:10">
+      <c r="K34" s="1">
+        <v>32</v>
+      </c>
+      <c r="L34" s="1">
+        <f t="shared" si="9"/>
+        <v>20.5</v>
+      </c>
+      <c r="M34" s="19">
+        <f t="shared" si="10"/>
+        <v>9.75</v>
+      </c>
+      <c r="N34" s="2">
+        <f t="shared" si="11"/>
+        <v>6</v>
+      </c>
+      <c r="O34" s="20">
+        <f t="shared" si="12"/>
+        <v>3.1</v>
+      </c>
+      <c r="P34" s="19">
+        <f t="shared" si="13"/>
+        <v>13.875</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16">
       <c r="A35" s="1">
         <v>33</v>
       </c>
@@ -1937,7 +2788,7 @@
         <v>414</v>
       </c>
       <c r="C35" s="13">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>123.76923076923077</v>
       </c>
       <c r="D35" s="12">
@@ -1949,27 +2800,50 @@
         <v>164</v>
       </c>
       <c r="F35" s="12">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>266.8</v>
       </c>
       <c r="G35" s="13">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>315.25</v>
       </c>
       <c r="H35" s="12">
-        <f t="shared" ref="H35:H62" si="14">14+A35+A35^2/10</f>
+        <f t="shared" ref="H35:H62" si="19">14+A35+A35^2/10</f>
         <v>155.9</v>
       </c>
       <c r="I35" s="13">
-        <f t="shared" ref="I35:I62" si="15">16+A35+1+A35^2/2</f>
+        <f t="shared" ref="I35:I62" si="20">16+A35+1+A35^2/2</f>
         <v>594.5</v>
       </c>
       <c r="J35" s="14">
         <f t="shared" si="8"/>
         <v>108906.65129511393</v>
       </c>
-    </row>
-    <row r="36" spans="1:10">
+      <c r="K35" s="1">
+        <v>33</v>
+      </c>
+      <c r="L35" s="1">
+        <f t="shared" si="9"/>
+        <v>21</v>
+      </c>
+      <c r="M35" s="19">
+        <f t="shared" si="10"/>
+        <v>10</v>
+      </c>
+      <c r="N35" s="2">
+        <f t="shared" si="11"/>
+        <v>6.166666666666667</v>
+      </c>
+      <c r="O35" s="20">
+        <f t="shared" si="12"/>
+        <v>3.2</v>
+      </c>
+      <c r="P35" s="19">
+        <f t="shared" si="13"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16">
       <c r="A36" s="1">
         <v>34</v>
       </c>
@@ -1978,7 +2852,7 @@
         <v>437.33333333333331</v>
       </c>
       <c r="C36" s="13">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>129.92307692307691</v>
       </c>
       <c r="D36" s="12">
@@ -1990,27 +2864,50 @@
         <v>172.44444444444446</v>
       </c>
       <c r="F36" s="12">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>281.2</v>
       </c>
       <c r="G36" s="13">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>333</v>
       </c>
       <c r="H36" s="12">
-        <f t="shared" si="14"/>
+        <f t="shared" si="19"/>
         <v>163.6</v>
       </c>
       <c r="I36" s="13">
-        <f t="shared" si="15"/>
+        <f t="shared" si="20"/>
         <v>629</v>
       </c>
       <c r="J36" s="14">
         <f t="shared" si="8"/>
         <v>115611.12106426293</v>
       </c>
-    </row>
-    <row r="37" spans="1:10">
+      <c r="K36" s="1">
+        <v>34</v>
+      </c>
+      <c r="L36" s="1">
+        <f t="shared" si="9"/>
+        <v>21.5</v>
+      </c>
+      <c r="M36" s="19">
+        <f t="shared" si="10"/>
+        <v>10.25</v>
+      </c>
+      <c r="N36" s="2">
+        <f t="shared" si="11"/>
+        <v>6.333333333333333</v>
+      </c>
+      <c r="O36" s="20">
+        <f t="shared" si="12"/>
+        <v>3.3</v>
+      </c>
+      <c r="P36" s="19">
+        <f t="shared" si="13"/>
+        <v>14.125</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16">
       <c r="A37" s="1">
         <v>35</v>
       </c>
@@ -2019,7 +2916,7 @@
         <v>461.33333333333331</v>
       </c>
       <c r="C37" s="13">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>136.23076923076923</v>
       </c>
       <c r="D37" s="12">
@@ -2031,27 +2928,50 @@
         <v>181.11111111111111</v>
       </c>
       <c r="F37" s="12">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>296</v>
       </c>
       <c r="G37" s="13">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>351.25</v>
       </c>
       <c r="H37" s="12">
-        <f t="shared" si="14"/>
+        <f t="shared" si="19"/>
         <v>171.5</v>
       </c>
       <c r="I37" s="13">
-        <f t="shared" si="15"/>
+        <f t="shared" si="20"/>
         <v>664.5</v>
       </c>
       <c r="J37" s="14">
         <f t="shared" si="8"/>
         <v>122518.69138926426</v>
       </c>
-    </row>
-    <row r="38" spans="1:10">
+      <c r="K37" s="1">
+        <v>35</v>
+      </c>
+      <c r="L37" s="1">
+        <f t="shared" si="9"/>
+        <v>22</v>
+      </c>
+      <c r="M37" s="19">
+        <f t="shared" si="10"/>
+        <v>10.5</v>
+      </c>
+      <c r="N37" s="2">
+        <f t="shared" si="11"/>
+        <v>6.5</v>
+      </c>
+      <c r="O37" s="20">
+        <f t="shared" si="12"/>
+        <v>3.4</v>
+      </c>
+      <c r="P37" s="19">
+        <f t="shared" si="13"/>
+        <v>14.25</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16">
       <c r="A38" s="1">
         <v>36</v>
       </c>
@@ -2060,7 +2980,7 @@
         <v>486</v>
       </c>
       <c r="C38" s="13">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>142.69230769230768</v>
       </c>
       <c r="D38" s="12">
@@ -2072,27 +2992,50 @@
         <v>190</v>
       </c>
       <c r="F38" s="12">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>311.2</v>
       </c>
       <c r="G38" s="13">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>370</v>
       </c>
       <c r="H38" s="12">
-        <f t="shared" si="14"/>
+        <f t="shared" si="19"/>
         <v>179.6</v>
       </c>
       <c r="I38" s="13">
-        <f t="shared" si="15"/>
+        <f t="shared" si="20"/>
         <v>701</v>
       </c>
       <c r="J38" s="14">
         <f t="shared" si="8"/>
         <v>129631.56929179345</v>
       </c>
-    </row>
-    <row r="39" spans="1:10">
+      <c r="K38" s="1">
+        <v>36</v>
+      </c>
+      <c r="L38" s="1">
+        <f t="shared" si="9"/>
+        <v>22.5</v>
+      </c>
+      <c r="M38" s="19">
+        <f t="shared" si="10"/>
+        <v>10.75</v>
+      </c>
+      <c r="N38" s="2">
+        <f t="shared" si="11"/>
+        <v>6.666666666666667</v>
+      </c>
+      <c r="O38" s="20">
+        <f t="shared" si="12"/>
+        <v>3.5</v>
+      </c>
+      <c r="P38" s="19">
+        <f t="shared" si="13"/>
+        <v>14.375</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16">
       <c r="A39" s="1">
         <v>37</v>
       </c>
@@ -2101,7 +3044,7 @@
         <v>511.33333333333331</v>
       </c>
       <c r="C39" s="13">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>149.30769230769232</v>
       </c>
       <c r="D39" s="12">
@@ -2113,27 +3056,50 @@
         <v>199.11111111111111</v>
       </c>
       <c r="F39" s="12">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>326.8</v>
       </c>
       <c r="G39" s="13">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>389.25</v>
       </c>
       <c r="H39" s="12">
-        <f t="shared" si="14"/>
+        <f t="shared" si="19"/>
         <v>187.9</v>
       </c>
       <c r="I39" s="13">
-        <f t="shared" si="15"/>
+        <f t="shared" si="20"/>
         <v>738.5</v>
       </c>
       <c r="J39" s="14">
         <f t="shared" si="8"/>
         <v>136953.56726772967</v>
       </c>
-    </row>
-    <row r="40" spans="1:10">
+      <c r="K39" s="1">
+        <v>37</v>
+      </c>
+      <c r="L39" s="1">
+        <f t="shared" si="9"/>
+        <v>23</v>
+      </c>
+      <c r="M39" s="19">
+        <f t="shared" si="10"/>
+        <v>11</v>
+      </c>
+      <c r="N39" s="2">
+        <f t="shared" si="11"/>
+        <v>6.833333333333333</v>
+      </c>
+      <c r="O39" s="20">
+        <f t="shared" si="12"/>
+        <v>3.6</v>
+      </c>
+      <c r="P39" s="19">
+        <f t="shared" si="13"/>
+        <v>14.5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16">
       <c r="A40" s="1">
         <v>38</v>
       </c>
@@ -2142,7 +3108,7 @@
         <v>537.33333333333326</v>
       </c>
       <c r="C40" s="13">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>156.07692307692309</v>
       </c>
       <c r="D40" s="12">
@@ -2154,27 +3120,50 @@
         <v>208.44444444444446</v>
       </c>
       <c r="F40" s="12">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>342.8</v>
       </c>
       <c r="G40" s="13">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>409</v>
       </c>
       <c r="H40" s="12">
-        <f t="shared" si="14"/>
+        <f t="shared" si="19"/>
         <v>196.4</v>
       </c>
       <c r="I40" s="13">
-        <f t="shared" si="15"/>
+        <f t="shared" si="20"/>
         <v>777</v>
       </c>
       <c r="J40" s="14">
         <f t="shared" si="8"/>
         <v>144491.29316328457</v>
       </c>
-    </row>
-    <row r="41" spans="1:10">
+      <c r="K40" s="1">
+        <v>38</v>
+      </c>
+      <c r="L40" s="1">
+        <f t="shared" si="9"/>
+        <v>23.5</v>
+      </c>
+      <c r="M40" s="19">
+        <f t="shared" si="10"/>
+        <v>11.25</v>
+      </c>
+      <c r="N40" s="2">
+        <f t="shared" si="11"/>
+        <v>7</v>
+      </c>
+      <c r="O40" s="20">
+        <f t="shared" si="12"/>
+        <v>3.7</v>
+      </c>
+      <c r="P40" s="19">
+        <f t="shared" si="13"/>
+        <v>14.625</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16">
       <c r="A41" s="1">
         <v>39</v>
       </c>
@@ -2183,7 +3172,7 @@
         <v>564</v>
       </c>
       <c r="C41" s="13">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>163</v>
       </c>
       <c r="D41" s="12">
@@ -2195,27 +3184,50 @@
         <v>218</v>
       </c>
       <c r="F41" s="12">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>359.2</v>
       </c>
       <c r="G41" s="13">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>429.25</v>
       </c>
       <c r="H41" s="12">
-        <f t="shared" si="14"/>
+        <f t="shared" si="19"/>
         <v>205.1</v>
       </c>
       <c r="I41" s="13">
-        <f t="shared" si="15"/>
+        <f t="shared" si="20"/>
         <v>816.5</v>
       </c>
       <c r="J41" s="14">
         <f t="shared" si="8"/>
         <v>152256.2363875373</v>
       </c>
-    </row>
-    <row r="42" spans="1:10">
+      <c r="K41" s="1">
+        <v>39</v>
+      </c>
+      <c r="L41" s="1">
+        <f t="shared" si="9"/>
+        <v>24</v>
+      </c>
+      <c r="M41" s="19">
+        <f t="shared" si="10"/>
+        <v>11.5</v>
+      </c>
+      <c r="N41" s="2">
+        <f t="shared" si="11"/>
+        <v>7.166666666666667</v>
+      </c>
+      <c r="O41" s="20">
+        <f t="shared" si="12"/>
+        <v>3.8</v>
+      </c>
+      <c r="P41" s="19">
+        <f t="shared" si="13"/>
+        <v>14.75</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16">
       <c r="A42" s="1">
         <v>40</v>
       </c>
@@ -2224,7 +3236,7 @@
         <v>591.33333333333337</v>
       </c>
       <c r="C42" s="13">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>170.07692307692309</v>
       </c>
       <c r="D42" s="12">
@@ -2236,27 +3248,50 @@
         <v>227.77777777777777</v>
       </c>
       <c r="F42" s="12">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>376</v>
       </c>
       <c r="G42" s="13">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>450</v>
       </c>
       <c r="H42" s="12">
-        <f t="shared" si="14"/>
+        <f t="shared" si="19"/>
         <v>214</v>
       </c>
       <c r="I42" s="13">
-        <f t="shared" si="15"/>
+        <f t="shared" si="20"/>
         <v>857</v>
       </c>
       <c r="J42" s="14">
         <f t="shared" si="8"/>
         <v>160268.43545600001</v>
       </c>
-    </row>
-    <row r="43" spans="1:10">
+      <c r="K42" s="1">
+        <v>40</v>
+      </c>
+      <c r="L42" s="1">
+        <f t="shared" si="9"/>
+        <v>24.5</v>
+      </c>
+      <c r="M42" s="19">
+        <f t="shared" si="10"/>
+        <v>11.75</v>
+      </c>
+      <c r="N42" s="2">
+        <f t="shared" si="11"/>
+        <v>7.333333333333333</v>
+      </c>
+      <c r="O42" s="20">
+        <f t="shared" si="12"/>
+        <v>3.9</v>
+      </c>
+      <c r="P42" s="19">
+        <f t="shared" si="13"/>
+        <v>14.875</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16">
       <c r="A43" s="1">
         <v>41</v>
       </c>
@@ -2265,7 +3300,7 @@
         <v>619.33333333333337</v>
       </c>
       <c r="C43" s="13">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>177.30769230769232</v>
       </c>
       <c r="D43" s="12">
@@ -2277,27 +3312,50 @@
         <v>237.77777777777777</v>
       </c>
       <c r="F43" s="12">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>393.2</v>
       </c>
       <c r="G43" s="13">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>471.25</v>
       </c>
       <c r="H43" s="12">
-        <f t="shared" si="14"/>
+        <f t="shared" si="19"/>
         <v>223.1</v>
       </c>
       <c r="I43" s="13">
-        <f t="shared" si="15"/>
+        <f t="shared" si="20"/>
         <v>898.5</v>
       </c>
       <c r="J43" s="14">
         <f t="shared" si="8"/>
         <v>168562.94210484295</v>
       </c>
-    </row>
-    <row r="44" spans="1:10">
+      <c r="K43" s="1">
+        <v>41</v>
+      </c>
+      <c r="L43" s="1">
+        <f t="shared" si="9"/>
+        <v>25</v>
+      </c>
+      <c r="M43" s="19">
+        <f t="shared" si="10"/>
+        <v>12</v>
+      </c>
+      <c r="N43" s="2">
+        <f t="shared" si="11"/>
+        <v>7.5</v>
+      </c>
+      <c r="O43" s="20">
+        <f t="shared" si="12"/>
+        <v>4</v>
+      </c>
+      <c r="P43" s="19">
+        <f t="shared" si="13"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16">
       <c r="A44" s="1">
         <v>42</v>
       </c>
@@ -2306,7 +3364,7 @@
         <v>648</v>
       </c>
       <c r="C44" s="13">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>184.69230769230768</v>
       </c>
       <c r="D44" s="12">
@@ -2318,27 +3376,50 @@
         <v>248</v>
       </c>
       <c r="F44" s="12">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>410.8</v>
       </c>
       <c r="G44" s="13">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>493</v>
       </c>
       <c r="H44" s="12">
-        <f t="shared" si="14"/>
+        <f t="shared" si="19"/>
         <v>232.4</v>
       </c>
       <c r="I44" s="13">
-        <f t="shared" si="15"/>
+        <f t="shared" si="20"/>
         <v>941</v>
       </c>
       <c r="J44" s="14">
         <f t="shared" si="8"/>
         <v>177201.24268108149</v>
       </c>
-    </row>
-    <row r="45" spans="1:10">
+      <c r="K44" s="1">
+        <v>42</v>
+      </c>
+      <c r="L44" s="1">
+        <f t="shared" si="9"/>
+        <v>25.5</v>
+      </c>
+      <c r="M44" s="19">
+        <f t="shared" si="10"/>
+        <v>12.25</v>
+      </c>
+      <c r="N44" s="2">
+        <f t="shared" si="11"/>
+        <v>7.666666666666667</v>
+      </c>
+      <c r="O44" s="20">
+        <f t="shared" si="12"/>
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="P44" s="19">
+        <f t="shared" si="13"/>
+        <v>15.125</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16">
       <c r="A45" s="1">
         <v>43</v>
       </c>
@@ -2347,7 +3428,7 @@
         <v>677.33333333333337</v>
       </c>
       <c r="C45" s="13">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>192.23076923076923</v>
       </c>
       <c r="D45" s="12">
@@ -2359,27 +3440,50 @@
         <v>258.44444444444446</v>
       </c>
       <c r="F45" s="12">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>428.8</v>
       </c>
       <c r="G45" s="13">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>515.25</v>
       </c>
       <c r="H45" s="12">
-        <f t="shared" si="14"/>
+        <f t="shared" si="19"/>
         <v>241.9</v>
       </c>
       <c r="I45" s="13">
-        <f t="shared" si="15"/>
+        <f t="shared" si="20"/>
         <v>984.5</v>
       </c>
       <c r="J45" s="14">
         <f t="shared" si="8"/>
         <v>186291.48676543732</v>
       </c>
-    </row>
-    <row r="46" spans="1:10">
+      <c r="K45" s="1">
+        <v>43</v>
+      </c>
+      <c r="L45" s="1">
+        <f t="shared" si="9"/>
+        <v>26</v>
+      </c>
+      <c r="M45" s="19">
+        <f t="shared" si="10"/>
+        <v>12.5</v>
+      </c>
+      <c r="N45" s="2">
+        <f t="shared" si="11"/>
+        <v>7.833333333333333</v>
+      </c>
+      <c r="O45" s="20">
+        <f t="shared" si="12"/>
+        <v>4.2</v>
+      </c>
+      <c r="P45" s="19">
+        <f t="shared" si="13"/>
+        <v>15.25</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16">
       <c r="A46" s="1">
         <v>44</v>
       </c>
@@ -2388,7 +3492,7 @@
         <v>707.33333333333337</v>
       </c>
       <c r="C46" s="13">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>199.92307692307693</v>
       </c>
       <c r="D46" s="12">
@@ -2400,27 +3504,50 @@
         <v>269.11111111111109</v>
       </c>
       <c r="F46" s="12">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>447.2</v>
       </c>
       <c r="G46" s="13">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>538</v>
       </c>
       <c r="H46" s="12">
-        <f t="shared" si="14"/>
+        <f t="shared" si="19"/>
         <v>251.6</v>
       </c>
       <c r="I46" s="13">
-        <f t="shared" si="15"/>
+        <f t="shared" si="20"/>
         <v>1029</v>
       </c>
       <c r="J46" s="14">
         <f t="shared" si="8"/>
         <v>196024.39706902555</v>
       </c>
-    </row>
-    <row r="47" spans="1:10">
+      <c r="K46" s="1">
+        <v>44</v>
+      </c>
+      <c r="L46" s="1">
+        <f t="shared" si="9"/>
+        <v>26.5</v>
+      </c>
+      <c r="M46" s="19">
+        <f t="shared" si="10"/>
+        <v>12.75</v>
+      </c>
+      <c r="N46" s="2">
+        <f t="shared" si="11"/>
+        <v>8</v>
+      </c>
+      <c r="O46" s="20">
+        <f t="shared" si="12"/>
+        <v>4.3</v>
+      </c>
+      <c r="P46" s="19">
+        <f t="shared" si="13"/>
+        <v>15.375</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16">
       <c r="A47" s="1">
         <v>45</v>
       </c>
@@ -2429,7 +3556,7 @@
         <v>738</v>
       </c>
       <c r="C47" s="13">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>207.76923076923077</v>
       </c>
       <c r="D47" s="12">
@@ -2441,27 +3568,50 @@
         <v>280</v>
       </c>
       <c r="F47" s="12">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>466</v>
       </c>
       <c r="G47" s="13">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>561.25</v>
       </c>
       <c r="H47" s="12">
-        <f t="shared" si="14"/>
+        <f t="shared" si="19"/>
         <v>261.5</v>
       </c>
       <c r="I47" s="13">
-        <f t="shared" si="15"/>
+        <f t="shared" si="20"/>
         <v>1074.5</v>
       </c>
       <c r="J47" s="14">
         <f t="shared" si="8"/>
         <v>206737.15861908518</v>
       </c>
-    </row>
-    <row r="48" spans="1:10">
+      <c r="K47" s="1">
+        <v>45</v>
+      </c>
+      <c r="L47" s="1">
+        <f t="shared" si="9"/>
+        <v>27</v>
+      </c>
+      <c r="M47" s="19">
+        <f t="shared" si="10"/>
+        <v>13</v>
+      </c>
+      <c r="N47" s="2">
+        <f t="shared" si="11"/>
+        <v>8.1666666666666679</v>
+      </c>
+      <c r="O47" s="20">
+        <f t="shared" si="12"/>
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="P47" s="19">
+        <f t="shared" si="13"/>
+        <v>15.5</v>
+      </c>
+    </row>
+    <row r="48" spans="1:16">
       <c r="A48" s="1">
         <v>46</v>
       </c>
@@ -2470,7 +3620,7 @@
         <v>769.33333333333337</v>
       </c>
       <c r="C48" s="13">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>215.76923076923077</v>
       </c>
       <c r="D48" s="12">
@@ -2482,27 +3632,50 @@
         <v>291.11111111111109</v>
       </c>
       <c r="F48" s="12">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>485.2</v>
       </c>
       <c r="G48" s="13">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>585</v>
       </c>
       <c r="H48" s="12">
-        <f t="shared" si="14"/>
+        <f t="shared" si="19"/>
         <v>271.60000000000002</v>
       </c>
       <c r="I48" s="13">
-        <f t="shared" si="15"/>
+        <f t="shared" si="20"/>
         <v>1121</v>
       </c>
       <c r="J48" s="14">
         <f t="shared" si="8"/>
         <v>219027.33154239375</v>
       </c>
-    </row>
-    <row r="49" spans="1:10">
+      <c r="K48" s="1">
+        <v>46</v>
+      </c>
+      <c r="L48" s="1">
+        <f t="shared" si="9"/>
+        <v>27.5</v>
+      </c>
+      <c r="M48" s="19">
+        <f t="shared" si="10"/>
+        <v>13.25</v>
+      </c>
+      <c r="N48" s="2">
+        <f t="shared" si="11"/>
+        <v>8.3333333333333321</v>
+      </c>
+      <c r="O48" s="20">
+        <f t="shared" si="12"/>
+        <v>4.5</v>
+      </c>
+      <c r="P48" s="19">
+        <f t="shared" si="13"/>
+        <v>15.625</v>
+      </c>
+    </row>
+    <row r="49" spans="1:16">
       <c r="A49" s="1">
         <v>47</v>
       </c>
@@ -2511,7 +3684,7 @@
         <v>801.33333333333337</v>
       </c>
       <c r="C49" s="13">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>223.92307692307693</v>
       </c>
       <c r="D49" s="12">
@@ -2523,27 +3696,50 @@
         <v>302.44444444444446</v>
       </c>
       <c r="F49" s="12">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>504.8</v>
       </c>
       <c r="G49" s="13">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>609.25</v>
       </c>
       <c r="H49" s="12">
-        <f t="shared" si="14"/>
+        <f t="shared" si="19"/>
         <v>281.89999999999998</v>
       </c>
       <c r="I49" s="13">
-        <f t="shared" si="15"/>
+        <f t="shared" si="20"/>
         <v>1168.5</v>
       </c>
       <c r="J49" s="14">
         <f t="shared" si="8"/>
         <v>233956.37600324146</v>
       </c>
-    </row>
-    <row r="50" spans="1:10">
+      <c r="K49" s="1">
+        <v>47</v>
+      </c>
+      <c r="L49" s="1">
+        <f t="shared" si="9"/>
+        <v>28</v>
+      </c>
+      <c r="M49" s="19">
+        <f t="shared" si="10"/>
+        <v>13.5</v>
+      </c>
+      <c r="N49" s="2">
+        <f t="shared" si="11"/>
+        <v>8.5</v>
+      </c>
+      <c r="O49" s="20">
+        <f t="shared" si="12"/>
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="P49" s="19">
+        <f t="shared" si="13"/>
+        <v>15.75</v>
+      </c>
+    </row>
+    <row r="50" spans="1:16">
       <c r="A50" s="1">
         <v>48</v>
       </c>
@@ -2552,7 +3748,7 @@
         <v>834</v>
       </c>
       <c r="C50" s="13">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>232.23076923076923</v>
       </c>
       <c r="D50" s="12">
@@ -2564,27 +3760,50 @@
         <v>314</v>
       </c>
       <c r="F50" s="12">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>524.79999999999995</v>
       </c>
       <c r="G50" s="13">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>634</v>
       </c>
       <c r="H50" s="12">
-        <f t="shared" si="14"/>
+        <f t="shared" si="19"/>
         <v>292.39999999999998</v>
       </c>
       <c r="I50" s="13">
-        <f t="shared" si="15"/>
+        <f t="shared" si="20"/>
         <v>1217</v>
       </c>
       <c r="J50" s="14">
         <f t="shared" si="8"/>
         <v>253414.01371742113</v>
       </c>
-    </row>
-    <row r="51" spans="1:10">
+      <c r="K50" s="1">
+        <v>48</v>
+      </c>
+      <c r="L50" s="1">
+        <f t="shared" si="9"/>
+        <v>28.5</v>
+      </c>
+      <c r="M50" s="19">
+        <f t="shared" si="10"/>
+        <v>13.75</v>
+      </c>
+      <c r="N50" s="2">
+        <f t="shared" si="11"/>
+        <v>8.6666666666666679</v>
+      </c>
+      <c r="O50" s="20">
+        <f t="shared" si="12"/>
+        <v>4.7</v>
+      </c>
+      <c r="P50" s="19">
+        <f t="shared" si="13"/>
+        <v>15.875</v>
+      </c>
+    </row>
+    <row r="51" spans="1:16">
       <c r="A51" s="1">
         <v>49</v>
       </c>
@@ -2593,7 +3812,7 @@
         <v>867.33333333333337</v>
       </c>
       <c r="C51" s="13">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>240.69230769230768</v>
       </c>
       <c r="D51" s="12">
@@ -2605,27 +3824,50 @@
         <v>325.77777777777777</v>
       </c>
       <c r="F51" s="12">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>545.20000000000005</v>
       </c>
       <c r="G51" s="13">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>659.25</v>
       </c>
       <c r="H51" s="12">
-        <f t="shared" si="14"/>
+        <f t="shared" si="19"/>
         <v>303.10000000000002</v>
       </c>
       <c r="I51" s="13">
-        <f t="shared" si="15"/>
+        <f t="shared" si="20"/>
         <v>1266.5</v>
       </c>
       <c r="J51" s="14">
         <f t="shared" si="8"/>
         <v>280771.79195448238</v>
       </c>
-    </row>
-    <row r="52" spans="1:10">
+      <c r="K51" s="1">
+        <v>49</v>
+      </c>
+      <c r="L51" s="1">
+        <f t="shared" si="9"/>
+        <v>29</v>
+      </c>
+      <c r="M51" s="19">
+        <f t="shared" si="10"/>
+        <v>14</v>
+      </c>
+      <c r="N51" s="2">
+        <f t="shared" si="11"/>
+        <v>8.8333333333333321</v>
+      </c>
+      <c r="O51" s="20">
+        <f t="shared" si="12"/>
+        <v>4.8</v>
+      </c>
+      <c r="P51" s="19">
+        <f t="shared" si="13"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="52" spans="1:16">
       <c r="A52" s="1">
         <v>50</v>
       </c>
@@ -2634,7 +3876,7 @@
         <v>901.33333333333337</v>
       </c>
       <c r="C52" s="13">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>249.30769230769232</v>
       </c>
       <c r="D52" s="12">
@@ -2646,27 +3888,50 @@
         <v>337.77777777777777</v>
       </c>
       <c r="F52" s="12">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>566</v>
       </c>
       <c r="G52" s="13">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>685</v>
       </c>
       <c r="H52" s="12">
-        <f t="shared" si="14"/>
+        <f t="shared" si="19"/>
         <v>314</v>
       </c>
       <c r="I52" s="13">
-        <f t="shared" si="15"/>
+        <f t="shared" si="20"/>
         <v>1317</v>
       </c>
       <c r="J52" s="14">
         <f t="shared" si="8"/>
         <v>322057.59403792792</v>
       </c>
-    </row>
-    <row r="53" spans="1:10">
+      <c r="K52" s="1">
+        <v>50</v>
+      </c>
+      <c r="L52" s="1">
+        <f t="shared" si="9"/>
+        <v>29.5</v>
+      </c>
+      <c r="M52" s="19">
+        <f t="shared" si="10"/>
+        <v>14.25</v>
+      </c>
+      <c r="N52" s="2">
+        <f t="shared" si="11"/>
+        <v>9</v>
+      </c>
+      <c r="O52" s="20">
+        <f t="shared" si="12"/>
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="P52" s="19">
+        <f t="shared" si="13"/>
+        <v>16.125</v>
+      </c>
+    </row>
+    <row r="53" spans="1:16">
       <c r="A53" s="1">
         <v>51</v>
       </c>
@@ -2675,7 +3940,7 @@
         <v>936</v>
       </c>
       <c r="C53" s="13">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>258.07692307692309</v>
       </c>
       <c r="D53" s="12">
@@ -2687,27 +3952,50 @@
         <v>350</v>
       </c>
       <c r="F53" s="12">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>587.20000000000005</v>
       </c>
       <c r="G53" s="13">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>711.25</v>
       </c>
       <c r="H53" s="12">
-        <f t="shared" si="14"/>
+        <f t="shared" si="19"/>
         <v>325.10000000000002</v>
       </c>
       <c r="I53" s="13">
-        <f t="shared" si="15"/>
+        <f t="shared" si="20"/>
         <v>1368.5</v>
       </c>
       <c r="J53" s="14">
         <f t="shared" si="8"/>
         <v>388070.16274974076</v>
       </c>
-    </row>
-    <row r="54" spans="1:10">
+      <c r="K53" s="1">
+        <v>51</v>
+      </c>
+      <c r="L53" s="1">
+        <f t="shared" si="9"/>
+        <v>30</v>
+      </c>
+      <c r="M53" s="19">
+        <f t="shared" si="10"/>
+        <v>14.5</v>
+      </c>
+      <c r="N53" s="2">
+        <f t="shared" si="11"/>
+        <v>9.1666666666666661</v>
+      </c>
+      <c r="O53" s="20">
+        <f t="shared" si="12"/>
+        <v>5</v>
+      </c>
+      <c r="P53" s="19">
+        <f t="shared" si="13"/>
+        <v>16.25</v>
+      </c>
+    </row>
+    <row r="54" spans="1:16">
       <c r="A54" s="1">
         <v>52</v>
       </c>
@@ -2716,7 +4004,7 @@
         <v>971.33333333333337</v>
       </c>
       <c r="C54" s="13">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>267</v>
       </c>
       <c r="D54" s="12">
@@ -2728,27 +4016,50 @@
         <v>362.44444444444446</v>
       </c>
       <c r="F54" s="12">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>608.79999999999995</v>
       </c>
       <c r="G54" s="13">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>738</v>
       </c>
       <c r="H54" s="12">
-        <f t="shared" si="14"/>
+        <f t="shared" si="19"/>
         <v>336.4</v>
       </c>
       <c r="I54" s="13">
-        <f t="shared" si="15"/>
+        <f t="shared" si="20"/>
         <v>1421</v>
       </c>
       <c r="J54" s="14">
         <f t="shared" si="8"/>
         <v>498192.65302936162</v>
       </c>
-    </row>
-    <row r="55" spans="1:10">
+      <c r="K54" s="1">
+        <v>52</v>
+      </c>
+      <c r="L54" s="1">
+        <f t="shared" si="9"/>
+        <v>30.5</v>
+      </c>
+      <c r="M54" s="19">
+        <f t="shared" si="10"/>
+        <v>14.75</v>
+      </c>
+      <c r="N54" s="2">
+        <f t="shared" si="11"/>
+        <v>9.3333333333333339</v>
+      </c>
+      <c r="O54" s="20">
+        <f t="shared" si="12"/>
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="P54" s="19">
+        <f t="shared" si="13"/>
+        <v>16.375</v>
+      </c>
+    </row>
+    <row r="55" spans="1:16">
       <c r="A55" s="1">
         <v>53</v>
       </c>
@@ -2757,7 +4068,7 @@
         <v>1007.3333333333334</v>
       </c>
       <c r="C55" s="13">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>276.07692307692309</v>
       </c>
       <c r="D55" s="12">
@@ -2769,27 +4080,50 @@
         <v>375.11111111111109</v>
       </c>
       <c r="F55" s="12">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>630.79999999999995</v>
       </c>
       <c r="G55" s="13">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>765.25</v>
       </c>
       <c r="H55" s="12">
-        <f t="shared" si="14"/>
+        <f t="shared" si="19"/>
         <v>347.9</v>
       </c>
       <c r="I55" s="13">
-        <f t="shared" si="15"/>
+        <f t="shared" si="20"/>
         <v>1474.5</v>
       </c>
       <c r="J55" s="14">
         <f t="shared" si="8"/>
         <v>687282.08348608389</v>
       </c>
-    </row>
-    <row r="56" spans="1:10">
+      <c r="K55" s="1">
+        <v>53</v>
+      </c>
+      <c r="L55" s="1">
+        <f t="shared" si="9"/>
+        <v>31</v>
+      </c>
+      <c r="M55" s="19">
+        <f t="shared" si="10"/>
+        <v>15</v>
+      </c>
+      <c r="N55" s="2">
+        <f t="shared" si="11"/>
+        <v>9.5</v>
+      </c>
+      <c r="O55" s="20">
+        <f t="shared" si="12"/>
+        <v>5.2</v>
+      </c>
+      <c r="P55" s="19">
+        <f t="shared" si="13"/>
+        <v>16.5</v>
+      </c>
+    </row>
+    <row r="56" spans="1:16">
       <c r="A56" s="1">
         <v>54</v>
       </c>
@@ -2798,7 +4132,7 @@
         <v>1044</v>
       </c>
       <c r="C56" s="13">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>285.30769230769232</v>
       </c>
       <c r="D56" s="12">
@@ -2810,27 +4144,50 @@
         <v>388</v>
       </c>
       <c r="F56" s="12">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>653.20000000000005</v>
       </c>
       <c r="G56" s="13">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>793</v>
       </c>
       <c r="H56" s="12">
-        <f t="shared" si="14"/>
+        <f t="shared" si="19"/>
         <v>359.6</v>
       </c>
       <c r="I56" s="13">
-        <f t="shared" si="15"/>
+        <f t="shared" si="20"/>
         <v>1529</v>
       </c>
       <c r="J56" s="14">
         <f t="shared" si="8"/>
         <v>1018136.1143836045</v>
       </c>
-    </row>
-    <row r="57" spans="1:10">
+      <c r="K56" s="1">
+        <v>54</v>
+      </c>
+      <c r="L56" s="1">
+        <f t="shared" si="9"/>
+        <v>31.5</v>
+      </c>
+      <c r="M56" s="19">
+        <f t="shared" si="10"/>
+        <v>15.25</v>
+      </c>
+      <c r="N56" s="2">
+        <f t="shared" si="11"/>
+        <v>9.6666666666666661</v>
+      </c>
+      <c r="O56" s="20">
+        <f t="shared" si="12"/>
+        <v>5.3</v>
+      </c>
+      <c r="P56" s="19">
+        <f t="shared" si="13"/>
+        <v>16.625</v>
+      </c>
+    </row>
+    <row r="57" spans="1:16">
       <c r="A57" s="1">
         <v>55</v>
       </c>
@@ -2839,7 +4196,7 @@
         <v>1081.3333333333335</v>
       </c>
       <c r="C57" s="13">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>294.69230769230768</v>
       </c>
       <c r="D57" s="12">
@@ -2851,27 +4208,50 @@
         <v>401.11111111111109</v>
       </c>
       <c r="F57" s="12">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>676</v>
       </c>
       <c r="G57" s="13">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>821.25</v>
       </c>
       <c r="H57" s="12">
-        <f t="shared" si="14"/>
+        <f t="shared" si="19"/>
         <v>371.5</v>
       </c>
       <c r="I57" s="13">
-        <f t="shared" si="15"/>
+        <f t="shared" si="20"/>
         <v>1584.5</v>
       </c>
       <c r="J57" s="14">
         <f t="shared" si="8"/>
         <v>1604088.2654978824</v>
       </c>
-    </row>
-    <row r="58" spans="1:10">
+      <c r="K57" s="1">
+        <v>55</v>
+      </c>
+      <c r="L57" s="1">
+        <f t="shared" si="9"/>
+        <v>32</v>
+      </c>
+      <c r="M57" s="19">
+        <f t="shared" si="10"/>
+        <v>15.5</v>
+      </c>
+      <c r="N57" s="2">
+        <f t="shared" si="11"/>
+        <v>9.8333333333333339</v>
+      </c>
+      <c r="O57" s="20">
+        <f t="shared" si="12"/>
+        <v>5.4</v>
+      </c>
+      <c r="P57" s="19">
+        <f t="shared" si="13"/>
+        <v>16.75</v>
+      </c>
+    </row>
+    <row r="58" spans="1:16">
       <c r="A58" s="1">
         <v>56</v>
       </c>
@@ -2880,7 +4260,7 @@
         <v>1119.3333333333333</v>
       </c>
       <c r="C58" s="13">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>304.23076923076923</v>
       </c>
       <c r="D58" s="12">
@@ -2892,27 +4272,50 @@
         <v>414.44444444444446</v>
       </c>
       <c r="F58" s="12">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>699.2</v>
       </c>
       <c r="G58" s="13">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>850</v>
       </c>
       <c r="H58" s="12">
-        <f t="shared" si="14"/>
+        <f t="shared" si="19"/>
         <v>383.6</v>
       </c>
       <c r="I58" s="13">
-        <f t="shared" si="15"/>
+        <f t="shared" si="20"/>
         <v>1641</v>
       </c>
       <c r="J58" s="14">
         <f t="shared" si="8"/>
         <v>2650023.6580336425</v>
       </c>
-    </row>
-    <row r="59" spans="1:10">
+      <c r="K58" s="1">
+        <v>56</v>
+      </c>
+      <c r="L58" s="1">
+        <f t="shared" si="9"/>
+        <v>32.5</v>
+      </c>
+      <c r="M58" s="19">
+        <f t="shared" si="10"/>
+        <v>15.75</v>
+      </c>
+      <c r="N58" s="2">
+        <f t="shared" si="11"/>
+        <v>10</v>
+      </c>
+      <c r="O58" s="20">
+        <f t="shared" si="12"/>
+        <v>5.5</v>
+      </c>
+      <c r="P58" s="19">
+        <f t="shared" si="13"/>
+        <v>16.875</v>
+      </c>
+    </row>
+    <row r="59" spans="1:16">
       <c r="A59" s="1">
         <v>57</v>
       </c>
@@ -2921,7 +4324,7 @@
         <v>1158</v>
       </c>
       <c r="C59" s="13">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>313.92307692307691</v>
       </c>
       <c r="D59" s="12">
@@ -2933,27 +4336,50 @@
         <v>428</v>
       </c>
       <c r="F59" s="12">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>722.8</v>
       </c>
       <c r="G59" s="13">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>879.25</v>
       </c>
       <c r="H59" s="12">
-        <f t="shared" si="14"/>
+        <f t="shared" si="19"/>
         <v>395.9</v>
       </c>
       <c r="I59" s="13">
-        <f t="shared" si="15"/>
+        <f t="shared" si="20"/>
         <v>1698.5</v>
       </c>
       <c r="J59" s="14">
         <f t="shared" si="8"/>
         <v>4526944.2242762595</v>
       </c>
-    </row>
-    <row r="60" spans="1:10">
+      <c r="K59" s="1">
+        <v>57</v>
+      </c>
+      <c r="L59" s="1">
+        <f t="shared" si="9"/>
+        <v>33</v>
+      </c>
+      <c r="M59" s="19">
+        <f t="shared" si="10"/>
+        <v>16</v>
+      </c>
+      <c r="N59" s="2">
+        <f t="shared" si="11"/>
+        <v>10.166666666666666</v>
+      </c>
+      <c r="O59" s="20">
+        <f t="shared" si="12"/>
+        <v>5.6</v>
+      </c>
+      <c r="P59" s="19">
+        <f t="shared" si="13"/>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="60" spans="1:16">
       <c r="A60" s="1">
         <v>58</v>
       </c>
@@ -2962,7 +4388,7 @@
         <v>1197.3333333333333</v>
       </c>
       <c r="C60" s="13">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>323.76923076923077</v>
       </c>
       <c r="D60" s="12">
@@ -2974,27 +4400,50 @@
         <v>441.77777777777777</v>
       </c>
       <c r="F60" s="12">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>746.8</v>
       </c>
       <c r="G60" s="13">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>909</v>
       </c>
       <c r="H60" s="12">
-        <f t="shared" si="14"/>
+        <f t="shared" si="19"/>
         <v>408.4</v>
       </c>
       <c r="I60" s="13">
-        <f t="shared" si="15"/>
+        <f t="shared" si="20"/>
         <v>1757</v>
       </c>
       <c r="J60" s="14">
         <f t="shared" si="8"/>
         <v>7907723.2288861386</v>
       </c>
-    </row>
-    <row r="61" spans="1:10">
+      <c r="K60" s="1">
+        <v>58</v>
+      </c>
+      <c r="L60" s="1">
+        <f t="shared" si="9"/>
+        <v>33.5</v>
+      </c>
+      <c r="M60" s="19">
+        <f t="shared" si="10"/>
+        <v>16.25</v>
+      </c>
+      <c r="N60" s="2">
+        <f t="shared" si="11"/>
+        <v>10.333333333333334</v>
+      </c>
+      <c r="O60" s="20">
+        <f t="shared" si="12"/>
+        <v>5.7</v>
+      </c>
+      <c r="P60" s="19">
+        <f t="shared" si="13"/>
+        <v>17.125</v>
+      </c>
+    </row>
+    <row r="61" spans="1:16">
       <c r="A61" s="1">
         <v>59</v>
       </c>
@@ -3003,7 +4452,7 @@
         <v>1237.3333333333333</v>
       </c>
       <c r="C61" s="13">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>333.76923076923077</v>
       </c>
       <c r="D61" s="12">
@@ -3015,27 +4464,50 @@
         <v>455.77777777777777</v>
       </c>
       <c r="F61" s="12">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>771.2</v>
       </c>
       <c r="G61" s="13">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>939.25</v>
       </c>
       <c r="H61" s="12">
-        <f t="shared" si="14"/>
+        <f t="shared" si="19"/>
         <v>421.1</v>
       </c>
       <c r="I61" s="13">
-        <f t="shared" si="15"/>
+        <f t="shared" si="20"/>
         <v>1816.5</v>
       </c>
       <c r="J61" s="14">
         <f t="shared" si="8"/>
         <v>14014611.600106845</v>
       </c>
-    </row>
-    <row r="62" spans="1:10">
+      <c r="K61" s="1">
+        <v>59</v>
+      </c>
+      <c r="L61" s="1">
+        <f t="shared" si="9"/>
+        <v>34</v>
+      </c>
+      <c r="M61" s="19">
+        <f t="shared" si="10"/>
+        <v>16.5</v>
+      </c>
+      <c r="N61" s="2">
+        <f t="shared" si="11"/>
+        <v>10.5</v>
+      </c>
+      <c r="O61" s="20">
+        <f t="shared" si="12"/>
+        <v>5.8</v>
+      </c>
+      <c r="P61" s="19">
+        <f t="shared" si="13"/>
+        <v>17.25</v>
+      </c>
+    </row>
+    <row r="62" spans="1:16">
       <c r="A62" s="1">
         <v>60</v>
       </c>
@@ -3044,7 +4516,7 @@
         <v>1278</v>
       </c>
       <c r="C62" s="13">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>343.92307692307691</v>
       </c>
       <c r="D62" s="12">
@@ -3056,24 +4528,64 @@
         <v>470</v>
       </c>
       <c r="F62" s="12">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>796</v>
       </c>
       <c r="G62" s="13">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>970</v>
       </c>
       <c r="H62" s="12">
-        <f t="shared" si="14"/>
+        <f t="shared" si="19"/>
         <v>434</v>
       </c>
       <c r="I62" s="13">
-        <f t="shared" si="15"/>
+        <f t="shared" si="20"/>
         <v>1877</v>
       </c>
       <c r="J62" s="14">
         <f t="shared" si="8"/>
         <v>25071109.06650478</v>
+      </c>
+      <c r="K62" s="1">
+        <v>60</v>
+      </c>
+      <c r="L62" s="1">
+        <f t="shared" si="9"/>
+        <v>34.5</v>
+      </c>
+      <c r="M62" s="19">
+        <f t="shared" si="10"/>
+        <v>16.75</v>
+      </c>
+      <c r="N62" s="2">
+        <f t="shared" si="11"/>
+        <v>10.666666666666666</v>
+      </c>
+      <c r="O62" s="20">
+        <f t="shared" si="12"/>
+        <v>5.9</v>
+      </c>
+      <c r="P62" s="19">
+        <f t="shared" si="13"/>
+        <v>17.375</v>
+      </c>
+    </row>
+    <row r="64" spans="1:16">
+      <c r="L64" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="M64" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="N64" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="O64" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="P64" s="19" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>